<commit_message>
Arreglo de bases del 2011, 2012
</commit_message>
<xml_diff>
--- a/AnalisisVariablesProyecto.xlsx
+++ b/AnalisisVariablesProyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\mineria de datos\ProyectoMineria1\Proyecto-analisis-y-clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E41F386-AAE7-45E6-ACE9-B605907EA7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D06A38E-4C5A-4D70-A0EC-85A4AEE2057A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27195" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="54">
   <si>
     <t>Depreg</t>
   </si>
@@ -181,13 +181,19 @@
   </si>
   <si>
     <t>Areagocu</t>
+  </si>
+  <si>
+    <t>NUNUHO</t>
+  </si>
+  <si>
+    <t>NUNUMU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +220,34 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -257,31 +291,52 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -564,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:K30"/>
+  <dimension ref="A4:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,598 +631,782 @@
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="11" max="11" width="27.7109375" customWidth="1"/>
+    <col min="15" max="15" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="E4" s="5" t="s">
+      <c r="C4" s="9"/>
+      <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="I4" s="5" t="s">
+      <c r="G4" s="9"/>
+      <c r="I4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="K4" s="9"/>
+      <c r="M4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="9"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="E5" s="5" t="s">
+      <c r="C5" s="5"/>
+      <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="I5" s="5" t="s">
+      <c r="G5" s="5"/>
+      <c r="I5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="K5" s="5"/>
+      <c r="M5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="E6" s="5" t="s">
+      <c r="C6" s="5"/>
+      <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="I6" s="5" t="s">
+      <c r="G6" s="5"/>
+      <c r="I6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="K6" s="5"/>
+      <c r="M6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="E7" s="5" t="s">
+      <c r="C7" s="5"/>
+      <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="I7" s="5" t="s">
+      <c r="G7" s="5"/>
+      <c r="I7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="K7" s="5"/>
+      <c r="M7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="E8" s="5" t="s">
+      <c r="C8" s="5"/>
+      <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="I8" s="5" t="s">
+      <c r="G8" s="5"/>
+      <c r="I8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="K8" s="5"/>
+      <c r="M8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="E9" s="5" t="s">
+      <c r="C9" s="5"/>
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="I9" s="5" t="s">
+      <c r="G9" s="5"/>
+      <c r="I9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="K9" s="5"/>
+      <c r="M9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="E10" s="5" t="s">
+      <c r="C10" s="5"/>
+      <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="I10" s="5" t="s">
+      <c r="G10" s="5"/>
+      <c r="I10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="K10" s="5"/>
+      <c r="M10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="E11" s="5" t="s">
+      <c r="C11" s="5"/>
+      <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="I11" s="8" t="s">
+      <c r="G11" s="5"/>
+      <c r="I11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="K11" s="7"/>
+      <c r="M11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11" s="14"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="E12" s="5" t="s">
+      <c r="C12" s="5"/>
+      <c r="E12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="I12" s="8" t="s">
+      <c r="G12" s="5"/>
+      <c r="I12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="K12" s="7"/>
+      <c r="M12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="O12" s="14"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="E13" s="5" t="s">
+      <c r="C13" s="5"/>
+      <c r="E13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="I13" s="6" t="s">
+      <c r="G13" s="5"/>
+      <c r="I13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="K13" s="6"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="E14" s="5" t="s">
+      <c r="C14" s="5"/>
+      <c r="E14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="I14" s="6" t="s">
+      <c r="G14" s="5"/>
+      <c r="I14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="7"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="K14" s="6"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="E15" s="5" t="s">
+      <c r="C15" s="5"/>
+      <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="I15" s="5" t="s">
+      <c r="G15" s="5"/>
+      <c r="I15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="K15" s="5"/>
+      <c r="M15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="E16" s="5" t="s">
+      <c r="C16" s="5"/>
+      <c r="E16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="I16" s="5" t="s">
+      <c r="G16" s="5"/>
+      <c r="I16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="K16" s="5"/>
+      <c r="M16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="E17" s="5" t="s">
+      <c r="C17" s="5"/>
+      <c r="E17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="I17" s="5" t="s">
+      <c r="G17" s="5"/>
+      <c r="I17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="K17" s="5"/>
+      <c r="M17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O17" s="5"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="E18" s="5" t="s">
+      <c r="C18" s="5"/>
+      <c r="E18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="I18" s="5" t="s">
+      <c r="G18" s="5"/>
+      <c r="I18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="K18" s="5"/>
+      <c r="M18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="E19" s="5" t="s">
+      <c r="C19" s="5"/>
+      <c r="E19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="I19" s="8" t="s">
+      <c r="G19" s="5"/>
+      <c r="I19" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J19" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="K19" s="8"/>
+      <c r="M19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="O19" s="8"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="E20" s="5" t="s">
+      <c r="C20" s="5"/>
+      <c r="E20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="I20" s="8" t="s">
+      <c r="G20" s="5"/>
+      <c r="I20" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J20" s="9" t="s">
+      <c r="J20" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="9"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="K20" s="8"/>
+      <c r="M20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O20" s="8"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="E21" s="5" t="s">
+      <c r="C21" s="5"/>
+      <c r="E21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="I21" s="6" t="s">
+      <c r="G21" s="5"/>
+      <c r="I21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="J21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K21" s="7"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="K21" s="6"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="E22" s="5" t="s">
+      <c r="C22" s="5"/>
+      <c r="E22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="I22" s="6" t="s">
+      <c r="G22" s="5"/>
+      <c r="I22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K22" s="7"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="K22" s="6"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="E23" s="6" t="s">
+      <c r="C23" s="5"/>
+      <c r="E23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="7"/>
-      <c r="I23" s="5" t="s">
+      <c r="G23" s="6"/>
+      <c r="I23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="K23" s="5"/>
+      <c r="M23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="E24" s="5" t="s">
+      <c r="C24" s="5"/>
+      <c r="E24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="I24" s="5" t="s">
+      <c r="G24" s="5"/>
+      <c r="I24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="K24" s="5"/>
+      <c r="M24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>2011</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="E25" s="2">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="E25" s="7">
         <v>2012</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="I25" s="5" t="s">
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="I25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I26" s="5" t="s">
+      <c r="K25" s="5"/>
+      <c r="M25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I27" s="8" t="s">
+      <c r="K26" s="5"/>
+      <c r="M26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="9" t="s">
+      <c r="J27" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="K27" s="9"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I28" s="6" t="s">
+      <c r="K27" s="8"/>
+      <c r="M27" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="N27" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="O27" s="16"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J28" s="7" t="s">
+      <c r="J28" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K28" s="7"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I29" s="6" t="s">
+      <c r="K28" s="6"/>
+      <c r="M28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="N28" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="O28" s="11"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J29" s="7" t="s">
+      <c r="J29" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K29" s="7"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I30" s="2">
+      <c r="K29" s="6"/>
+      <c r="M29" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I30" s="7">
         <v>2013</v>
       </c>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="M30" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M31" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="O31" s="6"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M32" s="7">
+        <v>2019</v>
+      </c>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="71">
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
+  <mergeCells count="100">
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
@@ -1184,18 +1423,49 @@
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J16:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>